<commit_message>
Ajuste no cadastro de busca por clique para diversos celulares
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub/appium/TestData/BancoDados.xlsx
+++ b/src/main/java/br/com/rsinet/hub/appium/TestData/BancoDados.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="142">
   <si>
     <t>Trocar@123</t>
   </si>
@@ -431,6 +431,33 @@
   </si>
   <si>
     <t>UWsvDH</t>
+  </si>
+  <si>
+    <t>Cqvx8f</t>
+  </si>
+  <si>
+    <t>yF8obI</t>
+  </si>
+  <si>
+    <t>ghjpyH</t>
+  </si>
+  <si>
+    <t>HS4laE</t>
+  </si>
+  <si>
+    <t>IrWuOM</t>
+  </si>
+  <si>
+    <t>TTufx1</t>
+  </si>
+  <si>
+    <t>JRcoO5</t>
+  </si>
+  <si>
+    <t>kAHF3U</t>
+  </si>
+  <si>
+    <t>QqKehg</t>
   </si>
 </sst>
 </file>
@@ -897,7 +924,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Ajuste com alguns erros na busca clique
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub/appium/TestData/BancoDados.xlsx
+++ b/src/main/java/br/com/rsinet/hub/appium/TestData/BancoDados.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="146">
   <si>
     <t>Trocar@123</t>
   </si>
@@ -458,6 +458,18 @@
   </si>
   <si>
     <t>QqKehg</t>
+  </si>
+  <si>
+    <t>YnEoRm</t>
+  </si>
+  <si>
+    <t>v5vrkU</t>
+  </si>
+  <si>
+    <t>opgp2P</t>
+  </si>
+  <si>
+    <t>WSOJpm</t>
   </si>
 </sst>
 </file>
@@ -924,7 +936,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>

</xml_diff>